<commit_message>
add scDesign3 and SimBPDD
</commit_message>
<xml_diff>
--- a/Chunk1-Data preparation/methods.xlsx
+++ b/Chunk1-Data preparation/methods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duohongrui/Desktop/simbenchmark/Chunk1-Data preparation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CAC9678-9491-144A-BBE7-4096D9110157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE0F383-A1C1-3C4C-8739-ABC93BD0F17B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30240" yWindow="1480" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{1C6D9BBE-D687-F842-A8B7-0BBC772AE287}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="98">
   <si>
     <t>Method</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -405,11 +405,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Class 6</t>
-  </si>
-  <si>
-    <t>Class 6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>scDesign3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Class 4</t>
+  </si>
+  <si>
+    <t>group.condition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch.condition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SimBPDD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>only return the well-fitted genes</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -504,7 +520,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -542,6 +558,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -858,11 +877,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F177C9-C3B1-E64E-99A7-B435FC89D838}">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView zoomScale="113" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+    <sheetView zoomScale="110" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1301,27 +1320,31 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="18">
+    <row r="20" spans="1:8" ht="38">
       <c r="A20" s="5" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="E20" s="2" t="s">
         <v>81</v>
       </c>
       <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="G20" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" ht="18">
       <c r="A21" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>88</v>
@@ -1329,9 +1352,7 @@
       <c r="C21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>49</v>
-      </c>
+      <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
         <v>81</v>
       </c>
@@ -1341,16 +1362,16 @@
     </row>
     <row r="22" spans="1:8" ht="18">
       <c r="A22" s="5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>81</v>
@@ -1361,7 +1382,7 @@
     </row>
     <row r="23" spans="1:8" ht="18">
       <c r="A23" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>87</v>
@@ -1369,7 +1390,9 @@
       <c r="C23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="2"/>
+      <c r="D23" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="E23" s="2" t="s">
         <v>81</v>
       </c>
@@ -1379,17 +1402,15 @@
     </row>
     <row r="24" spans="1:8" ht="18">
       <c r="A24" s="5" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>49</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D24" s="2"/>
       <c r="E24" s="2" t="s">
         <v>81</v>
       </c>
@@ -1397,64 +1418,72 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="38">
+    <row r="25" spans="1:8" ht="18">
       <c r="A25" s="5" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E25" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="F25" s="2"/>
-      <c r="G25" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" ht="18">
       <c r="A26" s="5" t="s">
-        <v>19</v>
+        <v>96</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" ht="18">
+    <row r="27" spans="1:8" ht="38">
       <c r="A27" s="5" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="2"/>
+      <c r="D27" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+      <c r="G27" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" ht="18">
       <c r="A28" s="5" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>7</v>
@@ -1467,17 +1496,15 @@
     </row>
     <row r="29" spans="1:8" ht="18">
       <c r="A29" s="5" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>80</v>
-      </c>
+      <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
@@ -1485,10 +1512,10 @@
     </row>
     <row r="30" spans="1:8" ht="18">
       <c r="A30" s="5" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>7</v>
@@ -1501,15 +1528,17 @@
     </row>
     <row r="31" spans="1:8" ht="18">
       <c r="A31" s="5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="2"/>
+      <c r="D31" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
@@ -1517,7 +1546,7 @@
     </row>
     <row r="32" spans="1:8" ht="18">
       <c r="A32" s="5" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>93</v>
@@ -1526,22 +1555,14 @@
         <v>7</v>
       </c>
       <c r="D32" s="2"/>
-      <c r="E32" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:8" ht="18">
       <c r="A33" s="5" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>93</v>
@@ -1550,25 +1571,17 @@
         <v>7</v>
       </c>
       <c r="D33" s="2"/>
-      <c r="E33" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" ht="18">
       <c r="A34" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>7</v>
@@ -1589,58 +1602,58 @@
     </row>
     <row r="35" spans="1:8" ht="18">
       <c r="A35" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>49</v>
-      </c>
+      <c r="D35" s="2"/>
       <c r="E35" s="2" t="s">
         <v>81</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G35" s="2"/>
+      <c r="G35" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="H35" s="2" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="18">
       <c r="A36" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>49</v>
-      </c>
+      <c r="D36" s="2"/>
       <c r="E36" s="2" t="s">
         <v>81</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G36" s="2"/>
+      <c r="G36" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="H36" s="2" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="18">
       <c r="A37" s="5" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>7</v>
@@ -1651,7 +1664,9 @@
       <c r="E37" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F37" s="2"/>
+      <c r="F37" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2" t="s">
         <v>81</v>
@@ -1659,10 +1674,10 @@
     </row>
     <row r="38" spans="1:8" ht="18">
       <c r="A38" s="5" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>7</v>
@@ -1673,7 +1688,9 @@
       <c r="E38" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F38" s="2"/>
+      <c r="F38" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2" t="s">
         <v>81</v>
@@ -1681,10 +1698,10 @@
     </row>
     <row r="39" spans="1:8" ht="18">
       <c r="A39" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>7</v>
@@ -1703,18 +1720,20 @@
     </row>
     <row r="40" spans="1:8" ht="18">
       <c r="A40" s="5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E40" s="2"/>
+      <c r="E40" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2" t="s">
@@ -1723,10 +1742,10 @@
     </row>
     <row r="41" spans="1:8" ht="18">
       <c r="A41" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>7</v>
@@ -1734,7 +1753,9 @@
       <c r="D41" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E41" s="2"/>
+      <c r="E41" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2" t="s">
@@ -1743,13 +1764,13 @@
     </row>
     <row r="42" spans="1:8" ht="18">
       <c r="A42" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>49</v>
@@ -1763,15 +1784,17 @@
     </row>
     <row r="43" spans="1:8" ht="18">
       <c r="A43" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D43" s="2"/>
+      <c r="D43" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
@@ -1781,19 +1804,57 @@
     </row>
     <row r="44" spans="1:8" ht="18">
       <c r="A44" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D44" s="2"/>
+      <c r="D44" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="18">
+      <c r="A45" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="18">
+      <c r="A46" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1805,10 +1866,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6822F7E0-AE7E-ED4E-97D1-B9217774D135}">
-  <dimension ref="A1:R44"/>
+  <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1817,20 +1878,20 @@
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.83203125" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
     <col min="8" max="8" width="12.83203125" customWidth="1"/>
     <col min="9" max="9" width="14.6640625" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.83203125" customWidth="1"/>
     <col min="13" max="13" width="19.1640625" customWidth="1"/>
     <col min="14" max="14" width="11.83203125" customWidth="1"/>
     <col min="15" max="15" width="12.5" customWidth="1"/>
     <col min="16" max="16" width="12.1640625" customWidth="1"/>
     <col min="17" max="17" width="12.83203125" customWidth="1"/>
-    <col min="18" max="18" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="34.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" ht="42" customHeight="1">
@@ -2507,52 +2568,54 @@
     </row>
     <row r="20" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A20" s="5" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
         <v>81</v>
       </c>
       <c r="D20" s="2"/>
-      <c r="E20" s="2">
-        <v>2</v>
-      </c>
-      <c r="F20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="G20" s="2"/>
-      <c r="H20" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
+      <c r="K20" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
+      <c r="R20" s="13"/>
     </row>
     <row r="21" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A21" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
         <v>81</v>
       </c>
       <c r="D21" s="2"/>
-      <c r="E21" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="E21" s="2">
+        <v>2</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
@@ -2565,22 +2628,24 @@
     </row>
     <row r="22" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A22" s="5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G22" s="4"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
+      <c r="I22" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
@@ -2593,7 +2658,7 @@
     </row>
     <row r="23" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A23" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
@@ -2602,16 +2667,14 @@
       <c r="D23" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E23" s="2">
-        <v>2</v>
-      </c>
-      <c r="F23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
-      <c r="J23" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
@@ -2623,19 +2686,25 @@
     </row>
     <row r="24" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A24" s="5" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="4" t="s">
-        <v>70</v>
-      </c>
+      <c r="C24" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="2">
+        <v>2</v>
+      </c>
+      <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
+      <c r="J24" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
@@ -2647,50 +2716,44 @@
     </row>
     <row r="25" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A25" s="5" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="B25" s="2"/>
-      <c r="C25" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
       <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="F25" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
-      <c r="K25" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L25" s="2" t="s">
-        <v>70</v>
-      </c>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
-      <c r="O25" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="P25" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q25" s="2" t="s">
-        <v>70</v>
-      </c>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
     </row>
     <row r="26" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A26" s="5" t="s">
-        <v>19</v>
+        <v>96</v>
       </c>
       <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
+      <c r="C26" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="E26" s="2">
+        <v>2</v>
+      </c>
       <c r="F26" s="4"/>
-      <c r="G26" s="2"/>
+      <c r="G26" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -2701,15 +2764,17 @@
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
-      <c r="R26" s="2"/>
+      <c r="R26" s="6" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="27" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A27" s="5" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>81</v>
@@ -2720,28 +2785,34 @@
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
+      <c r="K27" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
-      <c r="Q27" s="2"/>
+      <c r="O27" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="R27" s="2"/>
     </row>
     <row r="28" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A28" s="5" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B28" s="2"/>
-      <c r="C28" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="F28" s="4"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -2757,11 +2828,15 @@
     </row>
     <row r="29" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A29" s="5" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
+      <c r="C29" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
@@ -2772,20 +2847,14 @@
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
-      <c r="O29" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="P29" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q29" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
     </row>
     <row r="30" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A30" s="5" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
@@ -2811,12 +2880,10 @@
     </row>
     <row r="31" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A31" s="5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B31" s="2"/>
-      <c r="C31" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
@@ -2828,37 +2895,35 @@
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
-      <c r="Q31" s="2"/>
+      <c r="O31" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="R31" s="2"/>
     </row>
     <row r="32" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A32" s="5" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
-      <c r="H32" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
       <c r="J32" s="2"/>
-      <c r="K32" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="K32" s="2"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -2869,28 +2934,20 @@
     </row>
     <row r="33" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A33" s="5" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
-      <c r="H33" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
-      <c r="K33" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="K33" s="2"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -2901,7 +2958,7 @@
     </row>
     <row r="34" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A34" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
@@ -2935,7 +2992,7 @@
     </row>
     <row r="35" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A35" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
@@ -2947,18 +3004,16 @@
       <c r="E35" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F35" s="4" t="s">
-        <v>70</v>
-      </c>
+      <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I35" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="I35" s="2"/>
       <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
+      <c r="K35" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -2969,11 +3024,11 @@
     </row>
     <row r="36" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A36" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>81</v>
@@ -2981,9 +3036,7 @@
       <c r="E36" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F36" s="4" t="s">
-        <v>70</v>
-      </c>
+      <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2" t="s">
         <v>81</v>
@@ -2992,7 +3045,9 @@
         <v>81</v>
       </c>
       <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
+      <c r="K36" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -3003,20 +3058,28 @@
     </row>
     <row r="37" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A37" s="5" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
+      <c r="C37" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="D37" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E37" s="2"/>
+      <c r="E37" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="F37" s="4" t="s">
         <v>70</v>
       </c>
       <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
+      <c r="H37" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
@@ -3029,7 +3092,7 @@
     </row>
     <row r="38" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A38" s="5" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
@@ -3038,13 +3101,19 @@
       <c r="D38" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E38" s="2"/>
+      <c r="E38" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="F38" s="4" t="s">
         <v>70</v>
       </c>
       <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
+      <c r="H38" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
@@ -3057,12 +3126,10 @@
     </row>
     <row r="39" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A39" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B39" s="2"/>
-      <c r="C39" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
         <v>81</v>
       </c>
@@ -3085,7 +3152,7 @@
     </row>
     <row r="40" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A40" s="5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
@@ -3113,7 +3180,7 @@
     </row>
     <row r="41" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A41" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
@@ -3141,7 +3208,7 @@
     </row>
     <row r="42" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A42" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
@@ -3169,7 +3236,7 @@
     </row>
     <row r="43" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A43" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
@@ -3179,7 +3246,9 @@
         <v>81</v>
       </c>
       <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
+      <c r="F43" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
@@ -3195,7 +3264,7 @@
     </row>
     <row r="44" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A44" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
@@ -3205,7 +3274,9 @@
         <v>81</v>
       </c>
       <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
+      <c r="F44" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
@@ -3219,6 +3290,58 @@
       <c r="Q44" s="2"/>
       <c r="R44" s="2"/>
     </row>
+    <row r="45" spans="1:18" s="1" customFormat="1" ht="18">
+      <c r="A45" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+      <c r="Q45" s="2"/>
+      <c r="R45" s="2"/>
+    </row>
+    <row r="46" spans="1:18" s="1" customFormat="1" ht="18">
+      <c r="A46" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+      <c r="Q46" s="2"/>
+      <c r="R46" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="F1:G1"/>

</xml_diff>

<commit_message>
update trajectory and methods error
</commit_message>
<xml_diff>
--- a/Chunk1-Data preparation/methods.xlsx
+++ b/Chunk1-Data preparation/methods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duohongrui/Desktop/simbenchmark/Chunk1-Data preparation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE0F383-A1C1-3C4C-8739-ABC93BD0F17B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CD1131-9003-6B45-AA16-1AE76E0883AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30240" yWindow="1480" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{1C6D9BBE-D687-F842-A8B7-0BBC772AE287}"/>
   </bookViews>
@@ -1869,7 +1869,7 @@
   <dimension ref="A1:R46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
fix analysis codes and add SRTsim method
</commit_message>
<xml_diff>
--- a/Chunk1-Data preparation/methods.xlsx
+++ b/Chunk1-Data preparation/methods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duohongrui/Desktop/simbenchmark/Chunk1-Data preparation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DE356C-3A2A-0E45-BBCA-A3B5A16A680C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D93F94-9CD7-584C-90AD-B0028E6E50B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{1C6D9BBE-D687-F842-A8B7-0BBC772AE287}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{1C6D9BBE-D687-F842-A8B7-0BBC772AE287}"/>
   </bookViews>
   <sheets>
     <sheet name="Methods" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="122">
   <si>
     <t>Method</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -421,6 +421,114 @@
   </si>
   <si>
     <t>Publication Time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gamma-Poisson</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zero-inflated
+log-normal Poisson</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>log-linear model-based density estimation
+Gaussian copula</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zero-inflated negative binomial</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>negative binomial</t>
+  </si>
+  <si>
+    <t>(zero-inflated) Poisson
+negative binomial
+Gaussian copula</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bayesian
+negative binomial</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Optimisation framework</t>
+  </si>
+  <si>
+    <t>Generative adversarial network</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gamma-normal mixture model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gamma-multivariate
+hypergeometric model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Negative binomial model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gillespie’s stochastic simulation algorithm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Beta-Poisson</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gamma-Poisson
+(common biological coefficient variation)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Beta-Gamma-Poisson
+(common biological coefficient variation)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Beta-Gamma-Poisson
+(trended biological coefficient variation)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gamma-Poisson
+(trended biological coefficient variation)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>two-state kinetic model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pre-estimated noise mixture model and
+two drop-out models</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Poisson</t>
+  </si>
+  <si>
+    <t>negative binomial</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zero-inflated normal distribution</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>probabilistic model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Model</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -522,7 +630,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -563,12 +671,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -885,11 +1002,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F177C9-C3B1-E64E-99A7-B435FC89D838}">
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -898,15 +1015,16 @@
     <col min="2" max="2" width="25" style="1" customWidth="1"/>
     <col min="3" max="3" width="27.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="45.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27" customHeight="1">
+    <row r="1" spans="1:10" ht="27" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -919,23 +1037,26 @@
       <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18">
+    <row r="2" spans="1:10" ht="18">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -948,19 +1069,22 @@
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="E2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" ht="18">
+      <c r="I2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" ht="18">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -973,19 +1097,22 @@
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="E3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" ht="18">
+      <c r="I3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" ht="38">
       <c r="A4" s="5" t="s">
         <v>75</v>
       </c>
@@ -998,19 +1125,22 @@
       <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="E4" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" ht="18">
+      <c r="I4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" ht="38">
       <c r="A5" s="5" t="s">
         <v>76</v>
       </c>
@@ -1023,19 +1153,22 @@
       <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="E5" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" ht="18">
+      <c r="I5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" ht="38">
       <c r="A6" s="5" t="s">
         <v>77</v>
       </c>
@@ -1048,19 +1181,22 @@
       <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="E6" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" ht="18">
+      <c r="I6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" ht="18">
       <c r="A7" s="5" t="s">
         <v>78</v>
       </c>
@@ -1073,19 +1209,22 @@
       <c r="D7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="E7" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" ht="18">
+      <c r="I7" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" ht="38">
       <c r="A8" s="5" t="s">
         <v>79</v>
       </c>
@@ -1098,19 +1237,22 @@
       <c r="D8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="E8" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" ht="18">
+      <c r="I8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" ht="18">
       <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
@@ -1124,20 +1266,23 @@
         <v>7</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="G9" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" ht="38">
+      <c r="I9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" ht="38">
       <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
@@ -1151,20 +1296,23 @@
         <v>7</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="G10" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" ht="38">
+      <c r="I10" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" ht="38">
       <c r="A11" s="5" t="s">
         <v>25</v>
       </c>
@@ -1177,21 +1325,24 @@
       <c r="D11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="G11" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" ht="18">
+      <c r="I11" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" ht="18">
       <c r="A12" s="5" t="s">
         <v>39</v>
       </c>
@@ -1204,10 +1355,10 @@
       <c r="D12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="E12" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
         <v>81</v>
       </c>
@@ -1217,8 +1368,11 @@
       <c r="I12" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="18">
+      <c r="J12" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="18">
       <c r="A13" s="5" t="s">
         <v>40</v>
       </c>
@@ -1231,10 +1385,10 @@
       <c r="D13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="E13" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
         <v>81</v>
       </c>
@@ -1244,8 +1398,11 @@
       <c r="I13" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="18">
+      <c r="J13" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="18">
       <c r="A14" s="5" t="s">
         <v>44</v>
       </c>
@@ -1259,9 +1416,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="F14" s="2"/>
       <c r="G14" s="2" t="s">
         <v>81</v>
       </c>
@@ -1271,8 +1426,11 @@
       <c r="I14" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="18">
+      <c r="J14" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="18">
       <c r="A15" s="5" t="s">
         <v>42</v>
       </c>
@@ -1286,20 +1444,23 @@
         <v>7</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="G15" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="18">
+      <c r="H15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="18">
       <c r="A16" s="5" t="s">
         <v>43</v>
       </c>
@@ -1313,20 +1474,23 @@
         <v>7</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="G16" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="18">
+      <c r="H16" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="18">
       <c r="A17" s="5" t="s">
         <v>33</v>
       </c>
@@ -1340,18 +1504,21 @@
         <v>7</v>
       </c>
       <c r="E17" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G17" s="2"/>
+      <c r="G17" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="H17" s="2"/>
-      <c r="I17" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="18">
+      <c r="I17" s="2"/>
+      <c r="J17" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="19">
       <c r="A18" s="5" t="s">
         <v>36</v>
       </c>
@@ -1364,19 +1531,22 @@
       <c r="D18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G18" s="2"/>
+      <c r="G18" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="H18" s="2"/>
-      <c r="I18" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="18">
+      <c r="I18" s="2"/>
+      <c r="J18" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="19">
       <c r="A19" s="5" t="s">
         <v>37</v>
       </c>
@@ -1389,19 +1559,22 @@
       <c r="D19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G19" s="2"/>
+      <c r="G19" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="H19" s="2"/>
-      <c r="I19" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="18">
+      <c r="I19" s="2"/>
+      <c r="J19" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="18">
       <c r="A20" s="5" t="s">
         <v>32</v>
       </c>
@@ -1415,20 +1588,23 @@
         <v>46</v>
       </c>
       <c r="E20" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="18">
+      <c r="I20" s="2"/>
+      <c r="J20" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="18">
       <c r="A21" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="15">
+      <c r="B21" s="14">
         <v>2017</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -1437,17 +1613,18 @@
       <c r="D21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
-      <c r="I21" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="18">
+      <c r="I21" s="2"/>
+      <c r="J21" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="18">
       <c r="A22" s="5" t="s">
         <v>35</v>
       </c>
@@ -1461,16 +1638,19 @@
         <v>7</v>
       </c>
       <c r="E22" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="18">
+      <c r="I22" s="2"/>
+      <c r="J22" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="18">
       <c r="A23" s="5" t="s">
         <v>38</v>
       </c>
@@ -1483,15 +1663,18 @@
       <c r="D23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
-      <c r="I23" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="18">
+      <c r="I23" s="2"/>
+      <c r="J23" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="18">
       <c r="A24" s="5" t="s">
         <v>41</v>
       </c>
@@ -1504,15 +1687,18 @@
       <c r="D24" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
-      <c r="I24" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="18">
+      <c r="I24" s="2"/>
+      <c r="J24" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="18">
       <c r="A25" s="5" t="s">
         <v>12</v>
       </c>
@@ -1525,17 +1711,17 @@
       <c r="D25" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="F25" s="2"/>
       <c r="G25" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H25" s="2"/>
+      <c r="H25" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="I25" s="2"/>
-    </row>
-    <row r="26" spans="1:9" ht="18">
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="1:10" ht="18">
       <c r="A26" s="5" t="s">
         <v>13</v>
       </c>
@@ -1548,19 +1734,20 @@
       <c r="D26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="2"/>
+      <c r="F26" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="G26" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H26" s="10"/>
-      <c r="I26" s="2"/>
-    </row>
-    <row r="27" spans="1:9" ht="18">
+      <c r="H26" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I26" s="10"/>
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="1:10" ht="38">
       <c r="A27" s="5" t="s">
         <v>16</v>
       </c>
@@ -1573,19 +1760,22 @@
       <c r="D27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="G27" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H27" s="2"/>
+      <c r="H27" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="I27" s="2"/>
-    </row>
-    <row r="28" spans="1:9" ht="18">
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="1:10" ht="18">
       <c r="A28" s="5" t="s">
         <v>17</v>
       </c>
@@ -1598,17 +1788,20 @@
       <c r="D28" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="E28" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F28" s="2"/>
       <c r="G28" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H28" s="2"/>
+      <c r="H28" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="I28" s="2"/>
-    </row>
-    <row r="29" spans="1:9" ht="18">
+      <c r="J28" s="2"/>
+    </row>
+    <row r="29" spans="1:10" ht="18">
       <c r="A29" s="5" t="s">
         <v>26</v>
       </c>
@@ -1622,18 +1815,21 @@
         <v>7</v>
       </c>
       <c r="E29" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="G29" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H29" s="2"/>
+      <c r="H29" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="I29" s="2"/>
-    </row>
-    <row r="30" spans="1:9" ht="18">
+      <c r="J29" s="2"/>
+    </row>
+    <row r="30" spans="1:10" ht="18">
       <c r="A30" s="5" t="s">
         <v>28</v>
       </c>
@@ -1647,18 +1843,21 @@
         <v>7</v>
       </c>
       <c r="E30" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="G30" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H30" s="2"/>
+      <c r="H30" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="I30" s="2"/>
-    </row>
-    <row r="31" spans="1:9" ht="18">
+      <c r="J30" s="2"/>
+    </row>
+    <row r="31" spans="1:10" ht="18">
       <c r="A31" s="5" t="s">
         <v>20</v>
       </c>
@@ -1672,18 +1871,21 @@
         <v>7</v>
       </c>
       <c r="E31" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="G31" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H31" s="2"/>
+      <c r="H31" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="I31" s="2"/>
-    </row>
-    <row r="32" spans="1:9" ht="18">
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="1:10" ht="18">
       <c r="A32" s="5" t="s">
         <v>21</v>
       </c>
@@ -1696,19 +1898,20 @@
       <c r="D32" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E32" s="2"/>
+      <c r="F32" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="G32" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H32" s="2"/>
+      <c r="H32" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="I32" s="2"/>
-    </row>
-    <row r="33" spans="1:9" ht="38">
+      <c r="J32" s="2"/>
+    </row>
+    <row r="33" spans="1:10" ht="38">
       <c r="A33" s="5" t="s">
         <v>92</v>
       </c>
@@ -1721,19 +1924,22 @@
       <c r="D33" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="I33" s="2"/>
-    </row>
-    <row r="34" spans="1:9" ht="18">
+      <c r="G33" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J33" s="2"/>
+    </row>
+    <row r="34" spans="1:10" ht="38">
       <c r="A34" s="5" t="s">
         <v>15</v>
       </c>
@@ -1746,15 +1952,18 @@
       <c r="D34" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G34" s="2"/>
+      <c r="E34" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
-    </row>
-    <row r="35" spans="1:9" ht="18">
+      <c r="J34" s="2"/>
+    </row>
+    <row r="35" spans="1:10" ht="57">
       <c r="A35" s="5" t="s">
         <v>18</v>
       </c>
@@ -1767,17 +1976,20 @@
       <c r="D35" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E35" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G35" s="2"/>
+      <c r="G35" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
-    </row>
-    <row r="36" spans="1:9" ht="18">
+      <c r="J35" s="2"/>
+    </row>
+    <row r="36" spans="1:10" ht="18">
       <c r="A36" s="5" t="s">
         <v>27</v>
       </c>
@@ -1791,16 +2003,19 @@
         <v>7</v>
       </c>
       <c r="E36" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G36" s="2"/>
+      <c r="G36" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
-    </row>
-    <row r="37" spans="1:9" ht="18">
+      <c r="J36" s="2"/>
+    </row>
+    <row r="37" spans="1:10" ht="18">
       <c r="A37" s="5" t="s">
         <v>29</v>
       </c>
@@ -1813,15 +2028,18 @@
       <c r="D37" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G37" s="2"/>
+      <c r="E37" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
-    </row>
-    <row r="38" spans="1:9" ht="18">
+      <c r="J37" s="2"/>
+    </row>
+    <row r="38" spans="1:10" ht="18">
       <c r="A38" s="5" t="s">
         <v>45</v>
       </c>
@@ -1835,16 +2053,19 @@
         <v>46</v>
       </c>
       <c r="E38" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G38" s="2"/>
+      <c r="G38" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
-    </row>
-    <row r="39" spans="1:9" ht="18">
+      <c r="J38" s="2"/>
+    </row>
+    <row r="39" spans="1:10" ht="18">
       <c r="A39" s="5" t="s">
         <v>94</v>
       </c>
@@ -1858,16 +2079,19 @@
         <v>7</v>
       </c>
       <c r="E39" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F39" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G39" s="2"/>
+      <c r="G39" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
-    </row>
-    <row r="40" spans="1:9" ht="38">
+      <c r="J39" s="2"/>
+    </row>
+    <row r="40" spans="1:10" ht="38">
       <c r="A40" s="5" t="s">
         <v>22</v>
       </c>
@@ -1880,17 +2104,20 @@
       <c r="D40" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E40" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F40" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F40" s="2"/>
       <c r="G40" s="2"/>
-      <c r="H40" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="I40" s="2"/>
-    </row>
-    <row r="41" spans="1:9" ht="18">
+      <c r="H40" s="2"/>
+      <c r="I40" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J40" s="2"/>
+    </row>
+    <row r="41" spans="1:10" ht="18">
       <c r="A41" s="5" t="s">
         <v>19</v>
       </c>
@@ -1903,17 +2130,20 @@
       <c r="D41" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E41" s="2"/>
+      <c r="E41" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
-    </row>
-    <row r="42" spans="1:9" ht="18">
+      <c r="J41" s="2"/>
+    </row>
+    <row r="42" spans="1:10" ht="18">
       <c r="A42" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B42" s="15">
+      <c r="B42" s="14">
         <v>2017</v>
       </c>
       <c r="C42" s="2" t="s">
@@ -1927,12 +2157,13 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
-    </row>
-    <row r="43" spans="1:9" ht="18">
+      <c r="J42" s="2"/>
+    </row>
+    <row r="43" spans="1:10" ht="18">
       <c r="A43" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B43" s="15">
+      <c r="B43" s="14">
         <v>2017</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -1946,8 +2177,9 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
-    </row>
-    <row r="44" spans="1:9" ht="18">
+      <c r="J43" s="2"/>
+    </row>
+    <row r="44" spans="1:10" ht="38">
       <c r="A44" s="5" t="s">
         <v>23</v>
       </c>
@@ -1960,19 +2192,22 @@
       <c r="D44" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="E44" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F44" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
-    </row>
-    <row r="45" spans="1:9" ht="18">
+      <c r="J44" s="2"/>
+    </row>
+    <row r="45" spans="1:10" ht="18">
       <c r="A45" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B45" s="15">
+      <c r="B45" s="14">
         <v>2017</v>
       </c>
       <c r="C45" s="2" t="s">
@@ -1981,13 +2216,16 @@
       <c r="D45" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E45" s="2"/>
+      <c r="E45" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
-    </row>
-    <row r="46" spans="1:9" ht="18">
+      <c r="J45" s="2"/>
+    </row>
+    <row r="46" spans="1:10" ht="18">
       <c r="A46" s="5" t="s">
         <v>31</v>
       </c>
@@ -2005,6 +2243,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2017,7 +2256,7 @@
   <dimension ref="A1:R46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2058,10 +2297,10 @@
       <c r="E1" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="13"/>
+      <c r="G1" s="17"/>
       <c r="H1" s="7" t="s">
         <v>56</v>
       </c>
@@ -2074,10 +2313,10 @@
       <c r="K1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="M1" s="14"/>
+      <c r="M1" s="18"/>
       <c r="N1" s="7" t="s">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
add methods to excel
</commit_message>
<xml_diff>
--- a/Chunk1-Data preparation/methods.xlsx
+++ b/Chunk1-Data preparation/methods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duohongrui/Desktop/simbenchmark/Chunk1-Data preparation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D93F94-9CD7-584C-90AD-B0028E6E50B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B63D96-B7D6-A346-8525-DCEDCCF8CD03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{1C6D9BBE-D687-F842-A8B7-0BBC772AE287}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{1C6D9BBE-D687-F842-A8B7-0BBC772AE287}"/>
   </bookViews>
   <sheets>
     <sheet name="Methods" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="127">
   <si>
     <t>Method</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -529,6 +529,27 @@
   </si>
   <si>
     <t>Model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scMultiSim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kinetic model
+Beta-Poission model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scMultiSim-tree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRTsim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scDesign3-traj</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1002,11 +1023,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F177C9-C3B1-E64E-99A7-B435FC89D838}">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1490,68 +1511,72 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="18">
+    <row r="17" spans="1:10" ht="38">
       <c r="A17" s="5" t="s">
-        <v>33</v>
+        <v>124</v>
       </c>
       <c r="B17" s="2">
         <v>2022</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="F17" s="2" t="s">
+      <c r="E17" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>49</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
+      <c r="I17" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="J17" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="19">
+    <row r="18" spans="1:10" ht="38">
       <c r="A18" s="5" t="s">
-        <v>36</v>
+        <v>126</v>
       </c>
       <c r="B18" s="2">
-        <v>2019</v>
+        <v>2023</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>49</v>
+      <c r="E18" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
+      <c r="I18" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="J18" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="19">
+    <row r="19" spans="1:10" ht="18">
       <c r="A19" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B19" s="2">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>85</v>
@@ -1559,7 +1584,7 @@
       <c r="D19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>115</v>
       </c>
       <c r="F19" s="2" t="s">
@@ -1574,9 +1599,9 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="18">
+    <row r="20" spans="1:10" ht="19">
       <c r="A20" s="5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B20" s="2">
         <v>2019</v>
@@ -1585,27 +1610,29 @@
         <v>85</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>108</v>
+        <v>7</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G20" s="2"/>
+      <c r="G20" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="18">
+    <row r="21" spans="1:10" ht="19">
       <c r="A21" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="14">
-        <v>2017</v>
+        <v>37</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2021</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>85</v>
@@ -1613,11 +1640,15 @@
       <c r="D21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="2"/>
+      <c r="E21" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="F21" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G21" s="2"/>
+      <c r="G21" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2" t="s">
@@ -1626,19 +1657,19 @@
     </row>
     <row r="22" spans="1:10" ht="18">
       <c r="A22" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B22" s="2">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>85</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>49</v>
@@ -1652,9 +1683,9 @@
     </row>
     <row r="23" spans="1:10" ht="18">
       <c r="A23" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="2">
+        <v>34</v>
+      </c>
+      <c r="B23" s="14">
         <v>2017</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -1663,10 +1694,10 @@
       <c r="D23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -1676,10 +1707,10 @@
     </row>
     <row r="24" spans="1:10" ht="18">
       <c r="A24" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B24" s="2">
-        <v>2017</v>
+        <v>2021</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>85</v>
@@ -1688,9 +1719,11 @@
         <v>7</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="F24" s="2"/>
+        <v>109</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -1700,72 +1733,66 @@
     </row>
     <row r="25" spans="1:10" ht="18">
       <c r="A25" s="5" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="B25" s="2">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="E25" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="F25" s="2"/>
-      <c r="G25" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
       <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
+      <c r="J25" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="26" spans="1:10" ht="18">
       <c r="A26" s="5" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="B26" s="2">
         <v>2017</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="I26" s="10"/>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="1:10" ht="38">
+      <c r="E26" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="18">
       <c r="A27" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B27" s="2">
         <v>2016</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E27" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>48</v>
-      </c>
+      <c r="F27" s="2"/>
       <c r="G27" s="2" t="s">
         <v>81</v>
       </c>
@@ -1777,36 +1804,36 @@
     </row>
     <row r="28" spans="1:10" ht="18">
       <c r="A28" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B28" s="2">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="G28" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I28" s="2"/>
+      <c r="I28" s="10"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" ht="18">
+    <row r="29" spans="1:10" ht="38">
       <c r="A29" s="5" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B29" s="2">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>87</v>
@@ -1814,11 +1841,11 @@
       <c r="D29" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>97</v>
+      <c r="E29" s="16" t="s">
+        <v>103</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>81</v>
@@ -1831,10 +1858,10 @@
     </row>
     <row r="30" spans="1:10" ht="18">
       <c r="A30" s="5" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B30" s="2">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>87</v>
@@ -1843,11 +1870,9 @@
         <v>7</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>49</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="F30" s="2"/>
       <c r="G30" s="2" t="s">
         <v>81</v>
       </c>
@@ -1859,10 +1884,10 @@
     </row>
     <row r="31" spans="1:10" ht="18">
       <c r="A31" s="5" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B31" s="2">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>87</v>
@@ -1871,10 +1896,10 @@
         <v>7</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>81</v>
@@ -1887,10 +1912,10 @@
     </row>
     <row r="32" spans="1:10" ht="18">
       <c r="A32" s="5" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B32" s="2">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>87</v>
@@ -1898,9 +1923,11 @@
       <c r="D32" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E32" s="2"/>
+      <c r="E32" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="F32" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>81</v>
@@ -1911,12 +1938,12 @@
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10" ht="38">
+    <row r="33" spans="1:10" ht="18">
       <c r="A33" s="5" t="s">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="B33" s="2">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>87</v>
@@ -1925,111 +1952,117 @@
         <v>7</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>52</v>
+        <v>100</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="H33" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I33" s="2"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10" ht="38">
+    <row r="34" spans="1:10" ht="18">
       <c r="A34" s="5" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B34" s="2">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="G34" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H34" s="2"/>
+      <c r="H34" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10" ht="57">
+    <row r="35" spans="1:10" ht="38">
       <c r="A35" s="5" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
       <c r="B35" s="2">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J35" s="2"/>
+    </row>
+    <row r="36" spans="1:10" ht="38">
+      <c r="A36" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B36" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J36" s="2"/>
+    </row>
+    <row r="37" spans="1:10" ht="38">
+      <c r="A37" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-    </row>
-    <row r="36" spans="1:10" ht="18">
-      <c r="A36" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B36" s="2">
-        <v>2017</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-    </row>
-    <row r="37" spans="1:10" ht="18">
-      <c r="A37" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B37" s="2">
-        <v>2021</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="D37" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>101</v>
+      <c r="E37" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2" t="s">
@@ -2039,21 +2072,21 @@
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" ht="18">
+    <row r="38" spans="1:10" ht="57">
       <c r="A38" s="5" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="B38" s="2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>105</v>
+        <v>7</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>49</v>
@@ -2067,10 +2100,10 @@
     </row>
     <row r="39" spans="1:10" ht="18">
       <c r="A39" s="5" t="s">
-        <v>94</v>
+        <v>27</v>
       </c>
       <c r="B39" s="2">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>93</v>
@@ -2079,7 +2112,7 @@
         <v>7</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>48</v>
@@ -2091,12 +2124,12 @@
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10" ht="38">
+    <row r="40" spans="1:10" ht="18">
       <c r="A40" s="5" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B40" s="2">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>93</v>
@@ -2107,117 +2140,131 @@
       <c r="E40" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F40" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="H40" s="2"/>
-      <c r="I40" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
     <row r="41" spans="1:10" ht="18">
       <c r="A41" s="5" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="B41" s="2">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
+        <v>105</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
     </row>
     <row r="42" spans="1:10" ht="18">
       <c r="A42" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B42" s="14">
-        <v>2017</v>
+        <v>94</v>
+      </c>
+      <c r="B42" s="2">
+        <v>2021</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
+      <c r="E42" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
     </row>
     <row r="43" spans="1:10" ht="18">
       <c r="A43" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B43" s="14">
-        <v>2017</v>
+        <v>125</v>
+      </c>
+      <c r="B43" s="2">
+        <v>2023</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
+      <c r="F43" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
     </row>
     <row r="44" spans="1:10" ht="38">
       <c r="A44" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B44" s="2">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E44" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>80</v>
+      <c r="E44" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
+      <c r="I44" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="J44" s="2"/>
     </row>
     <row r="45" spans="1:10" ht="18">
       <c r="A45" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B45" s="14">
-        <v>2017</v>
+        <v>19</v>
+      </c>
+      <c r="B45" s="2">
+        <v>2018</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
@@ -2227,13 +2274,13 @@
     </row>
     <row r="46" spans="1:10" ht="18">
       <c r="A46" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B46" s="2">
-        <v>2019</v>
+        <v>8</v>
+      </c>
+      <c r="B46" s="14">
+        <v>2017</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>7</v>
@@ -2244,6 +2291,92 @@
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
+    </row>
+    <row r="47" spans="1:10" ht="18">
+      <c r="A47" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" s="14">
+        <v>2017</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+    </row>
+    <row r="48" spans="1:10" ht="38">
+      <c r="A48" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B48" s="2">
+        <v>2018</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+    </row>
+    <row r="49" spans="1:10" ht="18">
+      <c r="A49" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B49" s="14">
+        <v>2017</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+    </row>
+    <row r="50" spans="1:10" ht="18">
+      <c r="A50" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B50" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
add method information and fix scMultiSim execution code
</commit_message>
<xml_diff>
--- a/Chunk1-Data preparation/methods.xlsx
+++ b/Chunk1-Data preparation/methods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duohongrui/Desktop/simbenchmark/Chunk1-Data preparation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B63D96-B7D6-A346-8525-DCEDCCF8CD03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3BFB3C7-8A9E-9448-A5C6-B32E909507EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{1C6D9BBE-D687-F842-A8B7-0BBC772AE287}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{1C6D9BBE-D687-F842-A8B7-0BBC772AE287}"/>
   </bookViews>
   <sheets>
     <sheet name="Methods" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="128">
   <si>
     <t>Method</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -550,6 +550,10 @@
   </si>
   <si>
     <t>scDesign3-traj</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group.condition</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -651,7 +655,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -707,6 +711,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1025,9 +1032,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F177C9-C3B1-E64E-99A7-B435FC89D838}">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
+    <sheetView zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2386,10 +2393,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6822F7E0-AE7E-ED4E-97D1-B9217774D135}">
-  <dimension ref="A1:R46"/>
+  <dimension ref="A1:R50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3094,7 +3101,9 @@
         <v>81</v>
       </c>
       <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="F20" s="4" t="s">
         <v>70</v>
       </c>
@@ -3108,7 +3117,9 @@
       <c r="L20" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="M20" s="2"/>
+      <c r="M20" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
@@ -3117,52 +3128,52 @@
     </row>
     <row r="21" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A21" s="5" t="s">
-        <v>15</v>
+        <v>122</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2">
-        <v>2</v>
-      </c>
-      <c r="F21" s="2"/>
+      <c r="D21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="G21" s="2"/>
-      <c r="H21" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
+      <c r="K21" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
+      <c r="R21" s="11"/>
     </row>
     <row r="22" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A22" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
         <v>81</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G22" s="4"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="E22" s="2">
+        <v>2</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
@@ -3175,22 +3186,24 @@
     </row>
     <row r="23" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A23" s="5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G23" s="4"/>
       <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
+      <c r="I23" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
@@ -3203,7 +3216,7 @@
     </row>
     <row r="24" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A24" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
@@ -3212,16 +3225,14 @@
       <c r="D24" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E24" s="2">
-        <v>2</v>
-      </c>
-      <c r="F24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
-      <c r="J24" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
@@ -3233,19 +3244,25 @@
     </row>
     <row r="25" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A25" s="5" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="4" t="s">
-        <v>70</v>
-      </c>
+      <c r="C25" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E25" s="2">
+        <v>2</v>
+      </c>
+      <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
+      <c r="J25" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
@@ -3257,20 +3274,16 @@
     </row>
     <row r="26" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A26" s="5" t="s">
-        <v>94</v>
+        <v>45</v>
       </c>
       <c r="B26" s="2"/>
-      <c r="C26" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="2">
-        <v>2</v>
-      </c>
-      <c r="F26" s="4"/>
-      <c r="G26" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -3281,55 +3294,51 @@
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
-      <c r="R26" s="6" t="s">
-        <v>95</v>
-      </c>
+      <c r="R26" s="2"/>
     </row>
     <row r="27" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A27" s="5" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+        <v>81</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2">
+        <v>2</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
-      <c r="K27" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>70</v>
-      </c>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
-      <c r="O27" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="P27" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q27" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="R27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="28" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A28" s="5" t="s">
-        <v>19</v>
+        <v>125</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="4"/>
+      <c r="E28" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -3341,15 +3350,15 @@
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
-      <c r="R28" s="2"/>
+      <c r="R28" s="19"/>
     </row>
     <row r="29" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A29" s="5" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>81</v>
@@ -3360,28 +3369,34 @@
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
+      <c r="K29" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
-      <c r="Q29" s="2"/>
+      <c r="O29" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="R29" s="2"/>
     </row>
     <row r="30" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A30" s="5" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B30" s="2"/>
-      <c r="C30" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="F30" s="4"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -3397,11 +3412,15 @@
     </row>
     <row r="31" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A31" s="5" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
+      <c r="C31" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
@@ -3412,20 +3431,14 @@
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
-      <c r="O31" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="P31" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q31" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
     </row>
     <row r="32" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A32" s="5" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
@@ -3451,12 +3464,10 @@
     </row>
     <row r="33" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A33" s="5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B33" s="2"/>
-      <c r="C33" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
@@ -3468,37 +3479,35 @@
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
-      <c r="O33" s="2"/>
-      <c r="P33" s="2"/>
-      <c r="Q33" s="2"/>
+      <c r="O33" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="P33" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q33" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="R33" s="2"/>
     </row>
     <row r="34" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A34" s="5" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
       <c r="J34" s="2"/>
-      <c r="K34" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="K34" s="2"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -3509,28 +3518,20 @@
     </row>
     <row r="35" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A35" s="5" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>57</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
-      <c r="K35" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="K35" s="2"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -3541,7 +3542,7 @@
     </row>
     <row r="36" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A36" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
@@ -3575,11 +3576,11 @@
     </row>
     <row r="37" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A37" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>81</v>
@@ -3587,18 +3588,16 @@
       <c r="E37" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F37" s="4" t="s">
-        <v>70</v>
-      </c>
+      <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I37" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="I37" s="2"/>
       <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
+      <c r="K37" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -3609,11 +3608,11 @@
     </row>
     <row r="38" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A38" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>81</v>
@@ -3621,9 +3620,7 @@
       <c r="E38" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F38" s="4" t="s">
-        <v>70</v>
-      </c>
+      <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2" t="s">
         <v>81</v>
@@ -3632,7 +3629,9 @@
         <v>81</v>
       </c>
       <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
+      <c r="K38" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -3643,20 +3642,28 @@
     </row>
     <row r="39" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A39" s="5" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
+      <c r="C39" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="D39" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E39" s="2"/>
+      <c r="E39" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="F39" s="4" t="s">
         <v>70</v>
       </c>
       <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
+      <c r="H39" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
@@ -3669,7 +3676,7 @@
     </row>
     <row r="40" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A40" s="5" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
@@ -3678,13 +3685,19 @@
       <c r="D40" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E40" s="2"/>
+      <c r="E40" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="F40" s="4" t="s">
         <v>70</v>
       </c>
       <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
+      <c r="H40" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
@@ -3697,7 +3710,7 @@
     </row>
     <row r="41" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A41" s="5" t="s">
-        <v>37</v>
+        <v>124</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
@@ -3714,7 +3727,9 @@
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
+      <c r="K41" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -3725,26 +3740,32 @@
     </row>
     <row r="42" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A42" s="5" t="s">
-        <v>32</v>
+        <v>126</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="F42" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="G42" s="2"/>
+      <c r="G42" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
+      <c r="L42" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
       <c r="P42" s="2"/>
@@ -3753,12 +3774,10 @@
     </row>
     <row r="43" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A43" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B43" s="2"/>
-      <c r="C43" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="C43" s="2"/>
       <c r="D43" s="2" t="s">
         <v>81</v>
       </c>
@@ -3781,7 +3800,7 @@
     </row>
     <row r="44" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A44" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
@@ -3809,7 +3828,7 @@
     </row>
     <row r="45" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A45" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
@@ -3819,7 +3838,9 @@
         <v>81</v>
       </c>
       <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
+      <c r="F45" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
@@ -3835,7 +3856,7 @@
     </row>
     <row r="46" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A46" s="5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2" t="s">
@@ -3845,7 +3866,9 @@
         <v>81</v>
       </c>
       <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
+      <c r="F46" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
@@ -3859,6 +3882,114 @@
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
     </row>
+    <row r="47" spans="1:18" s="1" customFormat="1" ht="18">
+      <c r="A47" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E47" s="2"/>
+      <c r="F47" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
+      <c r="R47" s="2"/>
+    </row>
+    <row r="48" spans="1:18" s="1" customFormat="1" ht="18">
+      <c r="A48" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E48" s="2"/>
+      <c r="F48" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+      <c r="Q48" s="2"/>
+      <c r="R48" s="2"/>
+    </row>
+    <row r="49" spans="1:18" s="1" customFormat="1" ht="18">
+      <c r="A49" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2"/>
+      <c r="P49" s="2"/>
+      <c r="Q49" s="2"/>
+      <c r="R49" s="2"/>
+    </row>
+    <row r="50" spans="1:18" s="1" customFormat="1" ht="18">
+      <c r="A50" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2"/>
+      <c r="R50" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="F1:G1"/>

</xml_diff>

<commit_message>
add MoransI and fix codes
</commit_message>
<xml_diff>
--- a/Chunk1-Data preparation/methods.xlsx
+++ b/Chunk1-Data preparation/methods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duohongrui/Desktop/simbenchmark/Chunk1-Data preparation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33674DB1-BBE8-7F44-B928-CA60AC4B7623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D495C17-CFC1-5442-B6C7-8F1B339CC3FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{1C6D9BBE-D687-F842-A8B7-0BBC772AE287}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{1C6D9BBE-D687-F842-A8B7-0BBC772AE287}"/>
   </bookViews>
   <sheets>
     <sheet name="Methods" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="137">
   <si>
     <t>Method</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -399,9 +399,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Optimisation framework</t>
-  </si>
-  <si>
     <t>Gamma-multivariate
 hypergeometric model</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -414,10 +411,6 @@
     <t>Poisson</t>
   </si>
   <si>
-    <t>probabilistic model</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Model</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -462,23 +455,8 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>NB: Negative Binomial</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Gillespie’s stochastic simulation</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ZINB: zero-inflated normal distribution</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ZINB</t>
   </si>
   <si>
     <t>ZINB</t>
@@ -544,10 +522,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Poisson</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Noise mixture model +
 two drop-out models</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -581,10 +555,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Probabilistic model</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>GN</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -598,6 +568,22 @@
   </si>
   <si>
     <t>kinetic model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GAMLSS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZINB: zero-inflated negative binomial distribution</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Normal distribution</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>✓</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -605,7 +591,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -663,6 +649,12 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Segoe UI Symbol"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -748,8 +740,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1077,11 +1069,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F177C9-C3B1-E64E-99A7-B435FC89D838}">
-  <dimension ref="A1:K61"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1111,13 +1103,13 @@
         <v>76</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>8</v>
@@ -1149,10 +1141,10 @@
         <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2" t="s">
@@ -1180,10 +1172,10 @@
         <v>6</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
@@ -1211,10 +1203,10 @@
         <v>6</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
@@ -1242,10 +1234,10 @@
         <v>6</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
@@ -1273,10 +1265,10 @@
         <v>6</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
@@ -1304,10 +1296,10 @@
         <v>6</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
@@ -1335,10 +1327,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
@@ -1366,10 +1358,10 @@
         <v>6</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>74</v>
@@ -1399,13 +1391,13 @@
         <v>6</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>75</v>
@@ -1432,13 +1424,13 @@
         <v>6</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>75</v>
@@ -1465,10 +1457,10 @@
         <v>6</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2" t="s">
@@ -1498,10 +1490,10 @@
         <v>6</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
@@ -1531,10 +1523,10 @@
         <v>6</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>127</v>
+        <v>99</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
@@ -1564,13 +1556,13 @@
         <v>6</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>75</v>
@@ -1597,13 +1589,13 @@
         <v>6</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>75</v>
@@ -1618,7 +1610,7 @@
     </row>
     <row r="17" spans="1:11" ht="19">
       <c r="A17" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B17" s="2">
         <v>2022</v>
@@ -1630,13 +1622,13 @@
         <v>6</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>75</v>
@@ -1651,7 +1643,7 @@
     </row>
     <row r="18" spans="1:11" ht="38">
       <c r="A18" s="14" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B18" s="2">
         <v>2023</v>
@@ -1663,13 +1655,13 @@
         <v>6</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>75</v>
@@ -1696,13 +1688,13 @@
         <v>6</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>75</v>
@@ -1727,13 +1719,13 @@
         <v>6</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>75</v>
@@ -1758,13 +1750,13 @@
         <v>6</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>75</v>
@@ -1789,13 +1781,13 @@
         <v>45</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -1818,13 +1810,13 @@
         <v>6</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>108</v>
+        <v>127</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -1847,13 +1839,13 @@
         <v>6</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -1862,7 +1854,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="18">
+    <row r="25" spans="1:11" ht="21">
       <c r="A25" s="5" t="s">
         <v>37</v>
       </c>
@@ -1876,17 +1868,17 @@
         <v>6</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>111</v>
+        <v>135</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
-      <c r="K25" s="2" t="s">
-        <v>75</v>
+      <c r="K25" s="18" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="18">
@@ -1903,10 +1895,10 @@
         <v>6</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -1930,10 +1922,10 @@
         <v>6</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2" t="s">
@@ -1945,7 +1937,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" ht="19">
+    <row r="28" spans="1:11" ht="18">
       <c r="A28" s="5" t="s">
         <v>15</v>
       </c>
@@ -1958,14 +1950,14 @@
       <c r="D28" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E28" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="F28" s="18" t="s">
-        <v>108</v>
+      <c r="E28" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>75</v>
@@ -1990,10 +1982,10 @@
         <v>6</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2" t="s">
@@ -2019,13 +2011,13 @@
         <v>6</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>75</v>
@@ -2050,13 +2042,13 @@
         <v>6</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>75</v>
@@ -2081,13 +2073,13 @@
         <v>6</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>75</v>
@@ -2112,13 +2104,13 @@
         <v>6</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>75</v>
@@ -2143,13 +2135,13 @@
         <v>6</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>75</v>
@@ -2162,7 +2154,7 @@
     </row>
     <row r="35" spans="1:11" ht="19">
       <c r="A35" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B35" s="2">
         <v>2022</v>
@@ -2174,13 +2166,13 @@
         <v>6</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>75</v>
@@ -2205,10 +2197,10 @@
         <v>6</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2" t="s">
@@ -2232,13 +2224,13 @@
         <v>6</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>75</v>
@@ -2261,13 +2253,13 @@
         <v>6</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>91</v>
+        <v>135</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>75</v>
@@ -2290,10 +2282,10 @@
         <v>6</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2" t="s">
@@ -2317,13 +2309,13 @@
         <v>45</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>75</v>
@@ -2346,13 +2338,13 @@
         <v>6</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>75</v>
@@ -2363,7 +2355,7 @@
     </row>
     <row r="42" spans="1:11" ht="18">
       <c r="A42" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B42" s="2">
         <v>2023</v>
@@ -2375,13 +2367,13 @@
         <v>6</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>75</v>
@@ -2404,13 +2396,13 @@
         <v>6</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="2" t="s">
@@ -2432,10 +2424,10 @@
         <v>6</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>46</v>
@@ -2461,10 +2453,10 @@
         <v>6</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
@@ -2486,10 +2478,10 @@
         <v>6</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
@@ -2511,10 +2503,10 @@
         <v>6</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>127</v>
+        <v>99</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -2536,13 +2528,13 @@
         <v>6</v>
       </c>
       <c r="E48" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F48" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="F48" s="3" t="s">
-        <v>135</v>
-      </c>
       <c r="G48" s="2" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
@@ -2563,10 +2555,10 @@
         <v>6</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
@@ -2588,10 +2580,10 @@
         <v>6</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
@@ -2601,83 +2593,75 @@
     </row>
     <row r="52" spans="1:11" ht="20">
       <c r="A52" s="16" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="18">
       <c r="A53" s="19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B53" s="19"/>
       <c r="C53" s="19"/>
     </row>
     <row r="54" spans="1:11" ht="18">
       <c r="A54" s="19" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B54" s="19"/>
       <c r="C54" s="19"/>
     </row>
     <row r="55" spans="1:11" ht="18">
       <c r="A55" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B55" s="19"/>
       <c r="C55" s="19"/>
     </row>
     <row r="56" spans="1:11" ht="18">
       <c r="A56" s="19" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B56" s="19"/>
       <c r="C56" s="19"/>
     </row>
     <row r="57" spans="1:11" ht="18">
       <c r="A57" s="19" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="B57" s="19"/>
       <c r="C57" s="19"/>
     </row>
-    <row r="58" spans="1:11" ht="18">
-      <c r="A58" s="19" t="s">
+    <row r="58" spans="1:11" ht="38" customHeight="1">
+      <c r="A58" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="B58" s="20"/>
+      <c r="C58" s="20"/>
+    </row>
+    <row r="59" spans="1:11" ht="18">
+      <c r="A59" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="B58" s="19"/>
-      <c r="C58" s="19"/>
-    </row>
-    <row r="59" spans="1:11" ht="38" customHeight="1">
-      <c r="A59" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="B59" s="20"/>
-      <c r="C59" s="20"/>
+      <c r="B59" s="19"/>
+      <c r="C59" s="19"/>
     </row>
     <row r="60" spans="1:11" ht="18">
       <c r="A60" s="19" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B60" s="19"/>
       <c r="C60" s="19"/>
     </row>
-    <row r="61" spans="1:11" ht="18">
-      <c r="A61" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="B61" s="19"/>
-      <c r="C61" s="19"/>
-    </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A61:C61"/>
+  <mergeCells count="8">
+    <mergeCell ref="A60:C60"/>
     <mergeCell ref="A54:C54"/>
-    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="A59:C59"/>
     <mergeCell ref="A53:C53"/>
     <mergeCell ref="A55:C55"/>
     <mergeCell ref="A56:C56"/>
     <mergeCell ref="A57:C57"/>
     <mergeCell ref="A58:C58"/>
-    <mergeCell ref="A59:C59"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2688,8 +2672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6822F7E0-AE7E-ED4E-97D1-B9217774D135}">
   <dimension ref="A1:R50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3359,7 +3343,7 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>64</v>
@@ -3385,7 +3369,7 @@
     </row>
     <row r="20" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A20" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
@@ -3585,13 +3569,13 @@
     </row>
     <row r="27" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A27" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>64</v>
@@ -3997,7 +3981,7 @@
     </row>
     <row r="41" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A41" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
@@ -4027,7 +4011,7 @@
     </row>
     <row r="42" spans="1:18" s="1" customFormat="1" ht="18">
       <c r="A42" s="15" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
@@ -4035,7 +4019,7 @@
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F42" s="4" t="s">
         <v>64</v>

</xml_diff>